<commit_message>
dominated and equal in f#
</commit_message>
<xml_diff>
--- a/Multicriteria/bin/Debug/data.xlsx
+++ b/Multicriteria/bin/Debug/data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Cr1</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t>23.001</t>
+  </si>
+  <si>
+    <t>FFF</t>
+  </si>
+  <si>
+    <t>GGG</t>
   </si>
 </sst>
 </file>
@@ -386,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,6 +479,34 @@
       </c>
       <c r="D6" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>23</v>
+      </c>
+      <c r="C7">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>55</v>
+      </c>
+      <c r="D8">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -495,7 +529,7 @@
         <v>5</v>
       </c>
       <c r="B1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
         <v>6</v>

</xml_diff>